<commit_message>
added 7 test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/amazon.xlsx
+++ b/src/test/resources/amazon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROSHJOSE\IdeaProjects\Amazon_addToCart\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E1ADDF-5DD1-41EF-A84F-16E91670F9F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161C48C3-E9AE-44C7-94DE-5CF653F4D864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Scenario</t>
   </si>
@@ -48,6 +48,18 @@
   </si>
   <si>
     <t>Verify item is added to cart when add to cart button is clicked</t>
+  </si>
+  <si>
+    <t>Verify item can be deleted from cart and price is decreased</t>
+  </si>
+  <si>
+    <t>Verify items "No Results" is displayed for invalid product name</t>
+  </si>
+  <si>
+    <t>qqqqqqqqqqqq</t>
+  </si>
+  <si>
+    <t>Verify add to cart button</t>
   </si>
 </sst>
 </file>
@@ -399,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -435,6 +447,30 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added excel and assertion part
</commit_message>
<xml_diff>
--- a/src/test/resources/amazon.xlsx
+++ b/src/test/resources/amazon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROSHJOSE\IdeaProjects\Amazon_addToCart\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161C48C3-E9AE-44C7-94DE-5CF653F4D864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F877AC3-158E-4C7C-B9BF-DB1EF4E0FB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Scenario</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>Verify add to cart button</t>
+  </si>
+  <si>
+    <t>Assertion</t>
+  </si>
+  <si>
+    <t>Added to Cart</t>
   </si>
 </sst>
 </file>
@@ -411,35 +417,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="82.54296875" customWidth="1"/>
     <col min="2" max="2" width="15.453125" customWidth="1"/>
+    <col min="3" max="3" width="35.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -447,7 +460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -455,7 +468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -463,7 +476,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
all test cases are added
</commit_message>
<xml_diff>
--- a/src/test/resources/amazon.xlsx
+++ b/src/test/resources/amazon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROSHJOSE\IdeaProjects\Amazon_addToCart\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F877AC3-158E-4C7C-B9BF-DB1EF4E0FB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795046B2-D592-4F75-BF2F-D398E0F2D96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,6 +72,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;₹&quot;\ #,##0.00;[Red]&quot;₹&quot;\ \-#,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -101,8 +104,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,14 +424,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="82.54296875" customWidth="1"/>
     <col min="2" max="2" width="15.453125" customWidth="1"/>
-    <col min="3" max="3" width="35.1796875" customWidth="1"/>
+    <col min="3" max="3" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -459,6 +463,7 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">

</xml_diff>